<commit_message>
started parsing JKO data
</commit_message>
<xml_diff>
--- a/src/testData/fileFromJKO.xlsx
+++ b/src/testData/fileFromJKO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhartmann/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhartmann/Documents/project_elevate/src/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747BE2A4-6901-2A4D-B7EF-193BA2AC8CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ED4FB8-B2B3-1049-864B-C1F75A90601F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" xr2:uid="{A3C2142A-4549-314D-B15D-6669A783DCC3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{A3C2142A-4549-314D-B15D-6669A783DCC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +480,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F12" sqref="F12:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,6 +524,9 @@
       <c r="E2" t="s">
         <v>15</v>
       </c>
+      <c r="F2" s="1">
+        <v>45535</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -540,6 +544,9 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
+      <c r="F3" s="1">
+        <v>45535</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -557,6 +564,9 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
+      <c r="F4" s="1">
+        <v>45535</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -574,6 +584,9 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
+      <c r="F5" s="1">
+        <v>45534</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -591,6 +604,9 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
+      <c r="F6" s="1">
+        <v>45534</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -608,6 +624,9 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
+      <c r="F7" s="1">
+        <v>45534</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -625,6 +644,9 @@
       <c r="E8" t="s">
         <v>18</v>
       </c>
+      <c r="F8" s="1">
+        <v>45533</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -642,6 +664,9 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
+      <c r="F9" s="1">
+        <v>45533</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -659,6 +684,9 @@
       <c r="E10" t="s">
         <v>16</v>
       </c>
+      <c r="F10" s="1">
+        <v>45533</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -676,6 +704,9 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
+      <c r="F11" s="1">
+        <v>45533</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -693,6 +724,9 @@
       <c r="E12" t="s">
         <v>18</v>
       </c>
+      <c r="F12" s="1">
+        <v>45532</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -710,6 +744,9 @@
       <c r="E13" t="s">
         <v>19</v>
       </c>
+      <c r="F13" s="1">
+        <v>45532</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -727,6 +764,9 @@
       <c r="E14" t="s">
         <v>20</v>
       </c>
+      <c r="F14" s="1">
+        <v>45532</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -744,6 +784,9 @@
       <c r="E15" t="s">
         <v>21</v>
       </c>
+      <c r="F15" s="1">
+        <v>45532</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -760,6 +803,9 @@
       </c>
       <c r="E16" t="s">
         <v>22</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added completed date column to fake data
</commit_message>
<xml_diff>
--- a/src/testData/fileFromJKO.xlsx
+++ b/src/testData/fileFromJKO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhartmann/Documents/project_elevate/src/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018DA1C5-AEAE-2C45-8367-88CB78DCE9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3431FB6F-1C19-CF48-87B2-BE461F998FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{A3C2142A-4549-314D-B15D-6669A783DCC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t>Last Name</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Due Dt</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C891904-AD6F-0F41-A829-FDFB95408093}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +494,7 @@
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +513,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -530,8 +536,11 @@
       <c r="F2" s="1">
         <v>45535</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -550,8 +559,11 @@
       <c r="F3" s="1">
         <v>45535</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -570,8 +582,11 @@
       <c r="F4" s="1">
         <v>45535</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -590,8 +605,11 @@
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -607,11 +625,12 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="1">
-        <v>45595</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -630,8 +649,11 @@
       <c r="F7" s="1">
         <v>45534</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="1">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -650,8 +672,11 @@
       <c r="F8" s="1">
         <v>45533</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="1">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -670,8 +695,11 @@
       <c r="F9" s="1">
         <v>45533</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -690,8 +718,11 @@
       <c r="F10" s="1">
         <v>45533</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -710,8 +741,11 @@
       <c r="F11" s="1">
         <v>45533</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -730,8 +764,11 @@
       <c r="F12" s="1">
         <v>45532</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -750,8 +787,11 @@
       <c r="F13" s="1">
         <v>45532</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -770,8 +810,11 @@
       <c r="F14" s="1">
         <v>45532</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -790,8 +833,11 @@
       <c r="F15" s="1">
         <v>45532</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -810,8 +856,12 @@
       <c r="F16" s="1">
         <v>45532</v>
       </c>
+      <c r="G16" s="1">
+        <v>45536</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
parser now uses due date column to detect late courses
</commit_message>
<xml_diff>
--- a/src/testData/fileFromJKO.xlsx
+++ b/src/testData/fileFromJKO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhartmann/Documents/project_elevate/src/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3431FB6F-1C19-CF48-87B2-BE461F998FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11A62F-E846-624F-B19E-71E472416C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{A3C2142A-4549-314D-B15D-6669A783DCC3}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
UI now has standardized layouts and fonts
</commit_message>
<xml_diff>
--- a/src/testData/fileFromJKO.xlsx
+++ b/src/testData/fileFromJKO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhartmann/Documents/project_elevate/src/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11A62F-E846-624F-B19E-71E472416C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31757E3-B068-7349-9338-1A40EEB51B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{A3C2142A-4549-314D-B15D-6669A783DCC3}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
id build almost working
</commit_message>
<xml_diff>
--- a/src/testData/fileFromJKO.xlsx
+++ b/src/testData/fileFromJKO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhartmann/Documents/project_elevate/src/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nflet\Desktop\project_elevate\src\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31757E3-B068-7349-9338-1A40EEB51B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0CEB9B-CB8A-4470-BED1-A8DBAF13C659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{A3C2142A-4549-314D-B15D-6669A783DCC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A3C2142A-4549-314D-B15D-6669A783DCC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="28">
   <si>
     <t>Last Name</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Due Dt</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>RandomCourse</t>
   </si>
 </sst>
 </file>
@@ -483,18 +492,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C891904-AD6F-0F41-A829-FDFB95408093}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -540,7 +549,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -563,7 +572,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -586,7 +595,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -609,7 +618,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -630,7 +639,7 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -653,7 +662,7 @@
         <v>45505</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -676,16 +685,13 @@
         <v>45505</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
-        <v>4453245321</v>
-      </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
@@ -699,16 +705,13 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
-        <v>4453245321</v>
-      </c>
       <c r="D10" t="s">
         <v>14</v>
       </c>
@@ -722,16 +725,13 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
-        <v>4453245321</v>
-      </c>
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -745,16 +745,13 @@
         <v>45505</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>4453245321</v>
-      </c>
       <c r="D12" t="s">
         <v>14</v>
       </c>
@@ -768,16 +765,13 @@
         <v>45505</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13">
-        <v>5555555555</v>
-      </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
@@ -791,16 +785,13 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14">
-        <v>5555555555</v>
-      </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
@@ -814,16 +805,13 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
-        <v>5555555555</v>
-      </c>
       <c r="D15" t="s">
         <v>13</v>
       </c>
@@ -837,16 +825,13 @@
         <v>45536</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16">
-        <v>5555555555</v>
-      </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
@@ -858,6 +843,52 @@
       </c>
       <c r="G16" s="1">
         <v>45536</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>4453245321</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="1">
+        <v>36526</v>
+      </c>
+      <c r="G17" s="1">
+        <v>36527</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>5555555555</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1">
+        <v>36526</v>
+      </c>
+      <c r="G18" s="1">
+        <v>36161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>